<commit_message>
Added control group data
</commit_message>
<xml_diff>
--- a/Questionaire and data/MSc Dissertation_August 26, 2020_04.34.xlsx
+++ b/Questionaire and data/MSc Dissertation_August 26, 2020_04.34.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CommercialGamesDevelopment\Dissertation\MsC Dissertation\Questionaire and data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7602D400-5DAA-41F0-9F4E-9C7E42841BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F08865-3275-41B3-9516-676D028BC9BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSc Dissertation_August 26, 202" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MSc Dissertation_August 26, 202'!$B$1:$B$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MSc Dissertation_August 26, 202'!$B$1:$B$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
   <si>
     <t>Q14</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Average Highest Score</t>
+  </si>
+  <si>
+    <t>Overall Average</t>
   </si>
 </sst>
 </file>
@@ -906,14 +909,35 @@
               <c:f>'MSc Dissertation_August 26, 202'!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -924,14 +948,35 @@
               <c:f>'MSc Dissertation_August 26, 202'!$M$3:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>-1.7037127806056904E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6.0755202017543843E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>7.9999061186060046E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5861972799519325E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3.2363389222222219E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>9.611102083333331E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4137837556001382E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8570530265799982E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2537220053107157E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>8.7781430841584143E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1236,14 +1281,35 @@
               <c:f>'MSc Dissertation_August 26, 202'!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -1254,14 +1320,35 @@
               <c:f>'MSc Dissertation_August 26, 202'!$N$3:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>0.97499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.80701754385964908</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7931034482758621</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.88888888888888884</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91379310344827591</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95522388059701491</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.75247524752475248</c:v>
                 </c:pt>
               </c:numCache>
@@ -6028,7 +6115,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>4648200</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6064,7 +6151,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2804160</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6100,7 +6187,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>11975</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>20138</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6136,7 +6223,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6172,7 +6259,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>4974772</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6208,7 +6295,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>4648200</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>119743</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6534,32 +6621,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="92.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="96.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="62.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="71.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="96.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6606,7 +6692,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6644,7 +6730,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -6685,7 +6771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -6729,7 +6815,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -6773,7 +6859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -6814,7 +6900,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -6855,7 +6941,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -6899,7 +6985,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -6943,7 +7029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -6987,7 +7073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -7034,7 +7120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -7081,17 +7167,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -7100,7 +7186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -7109,7 +7195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -7117,12 +7203,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -7131,7 +7217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>70</v>
       </c>
@@ -7140,7 +7226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -7149,12 +7235,12 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -7163,7 +7249,7 @@
         <v>0.8161272267577635</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -7172,7 +7258,7 @@
         <v>0.8115900383141762</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -7181,91 +7267,81 @@
         <v>0.91725424601132277</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <f>AVERAGE(B30:B32)</f>
+        <v>0.84832383702775405</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <f>AVERAGE(M4,M7,M12)</f>
         <v>6.0300007360450068E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <f>AVERAGE(M3,M6,M8)</f>
         <v>5.1645288608931916E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <f>AVERAGE(M5,M9,M10,M11)</f>
         <v>3.9383004188573635E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>69</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <f>AVERAGE(O4,O7,O12)</f>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>70</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <f>AVERAGE(O3,O6,O8)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>71</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <f>AVERAGE(O5,O9,O10,O11)</f>
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B37" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="0.039383004"/>
-        <filter val="0.051645289"/>
-        <filter val="0.060300007"/>
-        <filter val="0.811590038"/>
-        <filter val="0.816127227"/>
-        <filter val="0.917254246"/>
-        <filter val="1"/>
-        <filter val="4"/>
-        <filter val="5"/>
-        <filter val="5.75"/>
-        <filter val="6"/>
-        <filter val="7"/>
-        <filter val="The First Person Shooter"/>
-        <filter val="Which prototype did you play?"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:B38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>